<commit_message>
Fix: Align tasks for Pedro with user 'Pedro Pascal' (Milestone)
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion.xlsx
+++ b/backend/plantilla_planificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_2BB1D69C5B1052CBE00865704B3088B35299F37C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{662EF23C-6C62-4E28-AD4D-3B5FE001A24D}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="11_2BB1D69C5B1052CBE00865704B3088B35299F37C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE98257D-A485-430C-9E8F-9676ACAF78A6}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>fecha</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Revision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro </t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -540,7 +543,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -563,7 +566,7 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Preparando deploy a Railway
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion.xlsx
+++ b/backend/plantilla_planificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="11_2BB1D69C5B1052CBE00865704B3088B35299F37C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE98257D-A485-430C-9E8F-9676ACAF78A6}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="11_2BB1D69C5B1052CBE00865704B3088B35299F37C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5B27691-E607-408E-AEE1-93417DA43E0D}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,12 +164,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,20 +475,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.9296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -587,6 +590,14 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>